<commit_message>
modifica del file Sprints
Ho aggiornato il file degli sprint
</commit_message>
<xml_diff>
--- a/Sprits.xlsx
+++ b/Sprits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\Progetti_SIW\Progetto_siw_RAVA[BAR]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32C9190-F9E2-413D-96ED-2E8FFB3FBC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635A7CC9-6AE1-4B08-8596-52A9BFA8F5F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Push</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Pietro</t>
   </si>
   <si>
-    <t>Note-&gt;le page con commento sono quelle che necessitano di concept</t>
-  </si>
-  <si>
     <t>19/05-26/05</t>
   </si>
   <si>
@@ -313,14 +310,53 @@
     <t>Terminati</t>
   </si>
   <si>
-    <t>Prenotazione tavolo</t>
+    <t>task: build del progetto</t>
+  </si>
+  <si>
+    <t>task:ordine domicilio e asporto</t>
+  </si>
+  <si>
+    <t>05/05-12/05</t>
+  </si>
+  <si>
+    <t>task: ??</t>
+  </si>
+  <si>
+    <t>codifica :Ordine a domicilio</t>
+  </si>
+  <si>
+    <t>codifica: Ordine da Asporto</t>
+  </si>
+  <si>
+    <t>codifica: Annulla e modifica Ordine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codifica: </t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Nome di chi insersice la nota</t>
+  </si>
+  <si>
+    <t>argomento</t>
+  </si>
+  <si>
+    <t>nota</t>
+  </si>
+  <si>
+    <t>Progettazione pagine</t>
+  </si>
+  <si>
+    <t>Le pagine con commento necessitano il concept, prima di proseguire nella loro implementazione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,19 +407,26 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -411,12 +454,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FF99"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -504,11 +565,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -516,70 +675,131 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -895,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,9 +1129,13 @@
     <col min="4" max="4" width="35.5546875" customWidth="1"/>
     <col min="7" max="7" width="23.109375" customWidth="1"/>
     <col min="8" max="8" width="29.5546875" customWidth="1"/>
+    <col min="12" max="12" width="28.77734375" customWidth="1"/>
+    <col min="13" max="13" width="29.21875" customWidth="1"/>
+    <col min="14" max="14" width="76.21875" customWidth="1"/>
+    <col min="15" max="17" width="55.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="26.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,191 +1148,306 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="25" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+    </row>
+    <row r="7" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="L8" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="45"/>
+      <c r="N8" s="46"/>
+    </row>
+    <row r="9" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49"/>
+    </row>
+    <row r="10" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>28</v>
+      <c r="L10" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="43"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="L12" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="17"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="22"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+    </row>
+    <row r="15" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="28"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="29"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+    </row>
+    <row r="17" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
+      <c r="H17" s="30"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+    </row>
+    <row r="18" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="H18" s="31"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+    </row>
+    <row r="19" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="32"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+    </row>
+    <row r="20" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="22"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F1:H6"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A20"/>
+  <mergeCells count="26">
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="L8:N9"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="M14:M15"/>
     <mergeCell ref="G12:H13"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A24"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>